<commit_message>
cadastro iptu e condominio
</commit_message>
<xml_diff>
--- a/inquilinos.xlsx
+++ b/inquilinos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,25 +444,31 @@
           <t>valor_aluguel</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>valor_iptu</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>valor_condominio</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Luiz Fernando</t>
+          <t>dazin</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Joao</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>550</v>
+        <v>1500</v>
+      </c>
+      <c r="C2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D2" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>